<commit_message>
Deleted testing db files. Added bibliography from feedback in tutorial. Modified schedule to be more specific to my project.
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Dev\Python\Projects\UniProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719B3A69-456D-4961-A40D-86D3F4F22B6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85A2FC8-7538-4966-A14B-563D6C9C4D8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1550" yWindow="1540" windowWidth="16710" windowHeight="12940" xr2:uid="{43BAE722-E837-440D-B254-BAD5D7941610}"/>
+    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{43BAE722-E837-440D-B254-BAD5D7941610}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="3" r:id="rId1"/>
+    <sheet name="Schedule (TMA specific tasks)" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,88 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>oem</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{890AA4F6-4D3B-4278-AB8D-B44EBD0B12AF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Look into similar projects which may have been undertaken.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{58259BFD-C940-4D43-B828-CCA2AC04B8B1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Research into where I can find past premier league results and stats.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{FDBC948F-EFCE-405B-91EF-FF681801DA2D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Identify differences between Oracle and MySql because I have used Oracle a lot more than MySql. Look into Python modules which I might need but don't have experience with.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6A1D8E13-142A-4CFE-9CBC-AE567850134D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>This is the first part of the schedule. Choose an appropriate lifecycle and describe why the choice was made.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{412283C2-18CD-42DD-8442-ECB6A956AE6F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Look into starting to design the database for storage of the stats. </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
   <si>
     <t>3rd Feb</t>
   </si>
@@ -315,6 +236,33 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Identify the goals and contents of my project</t>
+  </si>
+  <si>
+    <t>Look into similar studies/project which may have been undertaken.</t>
+  </si>
+  <si>
+    <t>Research into where I can find past premier league results and stats.</t>
+  </si>
+  <si>
+    <t>Choose an appropriate lifecycle and describe why the choice was made.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify differences between Oracle and MySql because I have used Oracle a lot more than MySql. </t>
+  </si>
+  <si>
+    <t>Look into Python modules which I might need but don't have experience with.</t>
+  </si>
+  <si>
+    <t>Look into starting to design the database for storage of the data.</t>
+  </si>
+  <si>
+    <t>Set up Python project</t>
+  </si>
+  <si>
+    <t>Set up database installation</t>
   </si>
 </sst>
 </file>
@@ -325,7 +273,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm"/>
     <numFmt numFmtId="165" formatCode="dd\-mm"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,13 +308,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -994,20 +935,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE3D4A8-75EC-4DC4-8648-55C84B390801}">
-  <dimension ref="A1:AI61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7380636A-BB9E-4EB1-A980-C240023CA5E4}">
+  <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.81640625" style="1" customWidth="1"/>
-    <col min="2" max="34" width="5.54296875" customWidth="1"/>
+    <col min="1" max="1" width="99.85546875" style="1" customWidth="1"/>
+    <col min="2" max="34" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="75.75" x14ac:dyDescent="0.25">
       <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1052,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>33</v>
       </c>
@@ -1154,9 +1095,9 @@
       <c r="AH2" s="44"/>
       <c r="AI2" s="21"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
@@ -1193,9 +1134,9 @@
       <c r="AH3" s="25"/>
       <c r="AI3" s="21"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1232,9 +1173,9 @@
       <c r="AH4" s="25"/>
       <c r="AI4" s="21"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5"/>
@@ -1271,9 +1212,9 @@
       <c r="AH5" s="25"/>
       <c r="AI5" s="21"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="5"/>
@@ -1310,7 +1251,1572 @@
       <c r="AH6" s="25"/>
       <c r="AI6" s="21"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="24"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="24"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="24"/>
+      <c r="AG7" s="24"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="21"/>
+    </row>
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="21"/>
+    </row>
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="21"/>
+    </row>
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="21"/>
+    </row>
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="21"/>
+    </row>
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="24"/>
+      <c r="AG12" s="24"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="21"/>
+    </row>
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AE13" s="24"/>
+      <c r="AF13" s="24"/>
+      <c r="AG13" s="24"/>
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="21"/>
+    </row>
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="3">
+        <v>43935</v>
+      </c>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="22"/>
+      <c r="AG14" s="22"/>
+      <c r="AH14" s="23"/>
+      <c r="AI14" s="21"/>
+    </row>
+    <row r="15" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="21"/>
+    </row>
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="23"/>
+      <c r="AI16" s="21"/>
+    </row>
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="23"/>
+      <c r="AI17" s="21"/>
+    </row>
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22"/>
+      <c r="AH18" s="23"/>
+      <c r="AI18" s="21"/>
+    </row>
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+      <c r="AG19" s="22"/>
+      <c r="AH19" s="23"/>
+      <c r="AI19" s="21"/>
+    </row>
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="22"/>
+      <c r="AH20" s="23"/>
+      <c r="AI20" s="21"/>
+    </row>
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+      <c r="V21" s="22"/>
+      <c r="W21" s="22"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
+      <c r="AB21" s="22"/>
+      <c r="AC21" s="22"/>
+      <c r="AD21" s="22"/>
+      <c r="AE21" s="22"/>
+      <c r="AF21" s="22"/>
+      <c r="AG21" s="22"/>
+      <c r="AH21" s="23"/>
+      <c r="AI21" s="21"/>
+    </row>
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="22"/>
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="22"/>
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="22"/>
+      <c r="AD22" s="22"/>
+      <c r="AE22" s="22"/>
+      <c r="AF22" s="22"/>
+      <c r="AG22" s="22"/>
+      <c r="AH22" s="23"/>
+      <c r="AI22" s="21"/>
+    </row>
+    <row r="23" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="3">
+        <v>44019</v>
+      </c>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="22"/>
+      <c r="AB23" s="22"/>
+      <c r="AC23" s="22"/>
+      <c r="AD23" s="22"/>
+      <c r="AE23" s="22"/>
+      <c r="AF23" s="22"/>
+      <c r="AG23" s="22"/>
+      <c r="AH23" s="23"/>
+      <c r="AI23" s="21"/>
+    </row>
+    <row r="24" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="22"/>
+      <c r="Z24" s="22"/>
+      <c r="AA24" s="22"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="22"/>
+      <c r="AD24" s="22"/>
+      <c r="AE24" s="22"/>
+      <c r="AF24" s="22"/>
+      <c r="AG24" s="22"/>
+      <c r="AH24" s="23"/>
+      <c r="AI24" s="21"/>
+    </row>
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="22"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22"/>
+      <c r="AD25" s="22"/>
+      <c r="AE25" s="22"/>
+      <c r="AF25" s="22"/>
+      <c r="AG25" s="22"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="21"/>
+    </row>
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22"/>
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="22"/>
+      <c r="AH26" s="23"/>
+      <c r="AI26" s="21"/>
+    </row>
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22"/>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
+      <c r="AG27" s="22"/>
+      <c r="AH27" s="23"/>
+      <c r="AI27" s="21"/>
+    </row>
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="21"/>
+    </row>
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22"/>
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22"/>
+      <c r="AH29" s="23"/>
+      <c r="AI29" s="21"/>
+    </row>
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="22"/>
+      <c r="AB30" s="22"/>
+      <c r="AC30" s="22"/>
+      <c r="AD30" s="22"/>
+      <c r="AE30" s="22"/>
+      <c r="AF30" s="22"/>
+      <c r="AG30" s="22"/>
+      <c r="AH30" s="23"/>
+      <c r="AI30" s="21"/>
+    </row>
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="22"/>
+      <c r="AB31" s="22"/>
+      <c r="AC31" s="22"/>
+      <c r="AD31" s="22"/>
+      <c r="AE31" s="22"/>
+      <c r="AF31" s="22"/>
+      <c r="AG31" s="22"/>
+      <c r="AH31" s="23"/>
+      <c r="AI31" s="21"/>
+    </row>
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="22"/>
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="22"/>
+      <c r="AD32" s="22"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="22"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="23"/>
+      <c r="AI32" s="21"/>
+    </row>
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
+      <c r="AG33" s="22"/>
+      <c r="AH33" s="23"/>
+      <c r="AI33" s="21"/>
+    </row>
+    <row r="34" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31"/>
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="31"/>
+      <c r="AD34" s="31"/>
+      <c r="AE34" s="31"/>
+      <c r="AF34" s="31"/>
+      <c r="AG34" s="31"/>
+      <c r="AH34" s="32">
+        <v>44088</v>
+      </c>
+      <c r="AI34" s="21"/>
+    </row>
+    <row r="35" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="33"/>
+      <c r="Z35" s="33"/>
+      <c r="AA35" s="33"/>
+      <c r="AB35" s="33"/>
+      <c r="AC35" s="33"/>
+      <c r="AD35" s="33"/>
+      <c r="AE35" s="33"/>
+      <c r="AF35" s="33"/>
+      <c r="AG35" s="33"/>
+      <c r="AH35" s="34"/>
+      <c r="AI35" s="21"/>
+    </row>
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
+      <c r="W36" s="35"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="37"/>
+      <c r="Z36" s="37"/>
+      <c r="AA36" s="37"/>
+      <c r="AB36" s="37"/>
+      <c r="AC36" s="37"/>
+      <c r="AD36" s="37"/>
+      <c r="AE36" s="37"/>
+      <c r="AF36" s="37"/>
+      <c r="AG36" s="37"/>
+      <c r="AH36" s="38"/>
+      <c r="AI36" s="21"/>
+    </row>
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:H36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE3D4A8-75EC-4DC4-8648-55C84B390801}">
+  <dimension ref="A1:AI61"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="99.85546875" style="1" customWidth="1"/>
+    <col min="2" max="34" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42">
+        <v>43893</v>
+      </c>
+      <c r="G2" s="43"/>
+      <c r="H2" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="21"/>
+    </row>
+    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="21"/>
+    </row>
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="21"/>
+    </row>
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="21"/>
+    </row>
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="21"/>
+    </row>
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
@@ -1349,7 +2855,7 @@
       <c r="AH7" s="25"/>
       <c r="AI7" s="21"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>43</v>
       </c>
@@ -1388,7 +2894,7 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="21"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
@@ -1427,7 +2933,7 @@
       <c r="AH9" s="25"/>
       <c r="AI9" s="21"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>45</v>
       </c>
@@ -1466,7 +2972,7 @@
       <c r="AH10" s="25"/>
       <c r="AI10" s="21"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1507,7 +3013,7 @@
       <c r="AH11" s="23"/>
       <c r="AI11" s="21"/>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>51</v>
       </c>
@@ -1546,7 +3052,7 @@
       <c r="AH12" s="23"/>
       <c r="AI12" s="21"/>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>52</v>
       </c>
@@ -1585,7 +3091,7 @@
       <c r="AH13" s="23"/>
       <c r="AI13" s="21"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>53</v>
       </c>
@@ -1624,7 +3130,7 @@
       <c r="AH14" s="23"/>
       <c r="AI14" s="21"/>
     </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>54</v>
       </c>
@@ -1663,7 +3169,7 @@
       <c r="AH15" s="23"/>
       <c r="AI15" s="21"/>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -1702,7 +3208,7 @@
       <c r="AH16" s="23"/>
       <c r="AI16" s="21"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>66</v>
       </c>
@@ -1741,7 +3247,7 @@
       <c r="AH17" s="23"/>
       <c r="AI17" s="21"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>56</v>
       </c>
@@ -1780,7 +3286,7 @@
       <c r="AH18" s="23"/>
       <c r="AI18" s="21"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>47</v>
       </c>
@@ -1819,7 +3325,7 @@
       <c r="AH19" s="23"/>
       <c r="AI19" s="21"/>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
@@ -1860,7 +3366,7 @@
       <c r="AH20" s="23"/>
       <c r="AI20" s="21"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>57</v>
       </c>
@@ -1899,7 +3405,7 @@
       <c r="AH21" s="23"/>
       <c r="AI21" s="21"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>58</v>
       </c>
@@ -1938,7 +3444,7 @@
       <c r="AH22" s="23"/>
       <c r="AI22" s="21"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>59</v>
       </c>
@@ -1977,7 +3483,7 @@
       <c r="AH23" s="23"/>
       <c r="AI23" s="21"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>60</v>
       </c>
@@ -2016,7 +3522,7 @@
       <c r="AH24" s="23"/>
       <c r="AI24" s="21"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>61</v>
       </c>
@@ -2055,7 +3561,7 @@
       <c r="AH25" s="23"/>
       <c r="AI25" s="21"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>62</v>
       </c>
@@ -2094,7 +3600,7 @@
       <c r="AH26" s="23"/>
       <c r="AI26" s="21"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -2133,7 +3639,7 @@
       <c r="AH27" s="23"/>
       <c r="AI27" s="21"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>64</v>
       </c>
@@ -2172,7 +3678,7 @@
       <c r="AH28" s="23"/>
       <c r="AI28" s="21"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>65</v>
       </c>
@@ -2211,7 +3717,7 @@
       <c r="AH29" s="23"/>
       <c r="AI29" s="21"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>48</v>
       </c>
@@ -2250,7 +3756,7 @@
       <c r="AH30" s="23"/>
       <c r="AI30" s="21"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>36</v>
       </c>
@@ -2291,7 +3797,7 @@
       </c>
       <c r="AI31" s="21"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>46</v>
       </c>
@@ -2330,7 +3836,7 @@
       <c r="AH32" s="34"/>
       <c r="AI32" s="21"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>50</v>
       </c>
@@ -2369,7 +3875,7 @@
       <c r="AH33" s="34"/>
       <c r="AI33" s="21"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>50</v>
       </c>
@@ -2408,7 +3914,7 @@
       <c r="AH34" s="34"/>
       <c r="AI34" s="21"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>50</v>
       </c>
@@ -2447,7 +3953,7 @@
       <c r="AH35" s="34"/>
       <c r="AI35" s="21"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>50</v>
       </c>
@@ -2486,7 +3992,7 @@
       <c r="AH36" s="34"/>
       <c r="AI36" s="21"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>50</v>
       </c>
@@ -2525,7 +4031,7 @@
       <c r="AH37" s="34"/>
       <c r="AI37" s="21"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>50</v>
       </c>
@@ -2564,7 +4070,7 @@
       <c r="AH38" s="34"/>
       <c r="AI38" s="21"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>50</v>
       </c>
@@ -2603,7 +4109,7 @@
       <c r="AH39" s="34"/>
       <c r="AI39" s="21"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>49</v>
       </c>
@@ -2642,67 +4148,67 @@
       <c r="AH40" s="38"/>
       <c r="AI40" s="21"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H61" s="2"/>
     </row>
   </sheetData>
@@ -2712,6 +4218,5 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated lifecycle_options, schedule. Added project_description, task_list and notes from tutorial. Updated project_journal with today's work.
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Dev\Python\Projects\UniProject\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31039E4B-2B56-45F1-8216-BBA48BDED589}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25427FDA-6B5F-448B-A177-D664C8EECBF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{43BAE722-E837-440D-B254-BAD5D7941610}"/>
+    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{43BAE722-E837-440D-B254-BAD5D7941610}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -41,23 +41,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Rob:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Away 28th Feb to 1st March, possibly away 2nd and 3rd March with work.</t>
+          <t>Away 28th Feb to 1st March. Possibly away 2nd and 3rd March with work.</t>
         </r>
       </text>
     </comment>
@@ -66,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>3rd Feb</t>
   </si>
@@ -345,6 +334,9 @@
   </si>
   <si>
     <t>Create graphs to show the learning aspect of the algorithm</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -355,7 +347,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm"/>
     <numFmt numFmtId="165" formatCode="dd\-mm"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,13 +384,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -696,6 +681,9 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -704,9 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,23 +1022,23 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.81640625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="5.54296875" customWidth="1"/>
-    <col min="6" max="6" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.54296875" customWidth="1"/>
-    <col min="12" max="12" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="23" width="5.54296875" customWidth="1"/>
-    <col min="24" max="24" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="25" max="33" width="5.54296875" customWidth="1"/>
-    <col min="34" max="34" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.85546875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="5.5703125" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="33" width="5.5703125" customWidth="1"/>
+    <col min="34" max="34" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="75.75" x14ac:dyDescent="0.25">
       <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1157,19 +1142,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="E2" s="41" t="s">
+        <v>93</v>
+      </c>
       <c r="F2" s="42">
         <v>43893</v>
       </c>
       <c r="G2" s="43"/>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="46" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="43"/>
@@ -1200,7 +1187,7 @@
       <c r="AH2" s="44"/>
       <c r="AI2" s="21"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>68</v>
       </c>
@@ -1210,7 +1197,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="22"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="46"/>
+      <c r="H3" s="47"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
@@ -1239,7 +1226,7 @@
       <c r="AH3" s="25"/>
       <c r="AI3" s="21"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>77</v>
       </c>
@@ -1249,7 +1236,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="22"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="46"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
@@ -1278,7 +1265,7 @@
       <c r="AH4" s="25"/>
       <c r="AI4" s="21"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>70</v>
       </c>
@@ -1288,7 +1275,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="22"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="46"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
@@ -1317,7 +1304,7 @@
       <c r="AH5" s="25"/>
       <c r="AI5" s="21"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>78</v>
       </c>
@@ -1326,7 +1313,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="22"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="46"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -1355,7 +1342,7 @@
       <c r="AH6" s="25"/>
       <c r="AI6" s="21"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>76</v>
       </c>
@@ -1364,7 +1351,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="22"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="46"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -1393,7 +1380,7 @@
       <c r="AH7" s="25"/>
       <c r="AI7" s="21"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>69</v>
       </c>
@@ -1403,7 +1390,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="22"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="46"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -1432,7 +1419,7 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="21"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>79</v>
       </c>
@@ -1442,7 +1429,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="22"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="46"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -1471,7 +1458,7 @@
       <c r="AH9" s="25"/>
       <c r="AI9" s="21"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>71</v>
       </c>
@@ -1481,7 +1468,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="22"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="46"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
@@ -1510,7 +1497,7 @@
       <c r="AH10" s="25"/>
       <c r="AI10" s="21"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>80</v>
       </c>
@@ -1520,7 +1507,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="22"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="46"/>
+      <c r="H11" s="47"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
@@ -1549,7 +1536,7 @@
       <c r="AH11" s="25"/>
       <c r="AI11" s="21"/>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>81</v>
       </c>
@@ -1559,7 +1546,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="22"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="46"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
@@ -1588,7 +1575,7 @@
       <c r="AH12" s="25"/>
       <c r="AI12" s="21"/>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>82</v>
       </c>
@@ -1598,7 +1585,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="22"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="46"/>
+      <c r="H13" s="47"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -1627,7 +1614,7 @@
       <c r="AH13" s="25"/>
       <c r="AI13" s="21"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>45</v>
       </c>
@@ -1637,7 +1624,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="22"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="46"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
@@ -1666,7 +1653,7 @@
       <c r="AH14" s="25"/>
       <c r="AI14" s="21"/>
     </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -1676,7 +1663,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="46"/>
+      <c r="H15" s="47"/>
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
@@ -1707,7 +1694,7 @@
       <c r="AH15" s="23"/>
       <c r="AI15" s="21"/>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>73</v>
       </c>
@@ -1717,7 +1704,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="28"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="46"/>
+      <c r="H16" s="47"/>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1746,7 +1733,7 @@
       <c r="AH16" s="23"/>
       <c r="AI16" s="21"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -1756,7 +1743,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="28"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="46"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="2"/>
@@ -1785,7 +1772,7 @@
       <c r="AH17" s="23"/>
       <c r="AI17" s="21"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>72</v>
       </c>
@@ -1795,7 +1782,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="5"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="2"/>
@@ -1824,7 +1811,7 @@
       <c r="AH18" s="23"/>
       <c r="AI18" s="21"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -1834,7 +1821,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="5"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="46"/>
+      <c r="H19" s="47"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1863,7 +1850,7 @@
       <c r="AH19" s="23"/>
       <c r="AI19" s="21"/>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>84</v>
       </c>
@@ -1873,7 +1860,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="5"/>
       <c r="G20" s="28"/>
-      <c r="H20" s="46"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="28"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1902,7 +1889,7 @@
       <c r="AH20" s="23"/>
       <c r="AI20" s="21"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>85</v>
       </c>
@@ -1912,7 +1899,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="46"/>
+      <c r="H21" s="47"/>
       <c r="I21" s="28"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1941,7 +1928,7 @@
       <c r="AH21" s="23"/>
       <c r="AI21" s="21"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>91</v>
       </c>
@@ -1951,7 +1938,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="46"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
       <c r="K22" s="5"/>
@@ -1980,7 +1967,7 @@
       <c r="AH22" s="23"/>
       <c r="AI22" s="21"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>82</v>
       </c>
@@ -1990,7 +1977,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="46"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="5"/>
       <c r="J23" s="28"/>
       <c r="K23" s="5"/>
@@ -2019,7 +2006,7 @@
       <c r="AH23" s="23"/>
       <c r="AI23" s="21"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>47</v>
       </c>
@@ -2029,7 +2016,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="46"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="5"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
@@ -2058,7 +2045,7 @@
       <c r="AH24" s="23"/>
       <c r="AI24" s="21"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>35</v>
       </c>
@@ -2068,7 +2055,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="46"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
@@ -2099,7 +2086,7 @@
       <c r="AH25" s="23"/>
       <c r="AI25" s="21"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>86</v>
       </c>
@@ -2109,7 +2096,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="46"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
@@ -2138,8 +2125,8 @@
       <c r="AH26" s="23"/>
       <c r="AI26" s="21"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="48" t="s">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="22"/>
@@ -2148,7 +2135,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="46"/>
+      <c r="H27" s="47"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
@@ -2177,8 +2164,8 @@
       <c r="AH27" s="23"/>
       <c r="AI27" s="21"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>90</v>
       </c>
       <c r="B28" s="22"/>
@@ -2187,7 +2174,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="46"/>
+      <c r="H28" s="47"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -2216,7 +2203,7 @@
       <c r="AH28" s="23"/>
       <c r="AI28" s="21"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>87</v>
       </c>
@@ -2226,7 +2213,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="46"/>
+      <c r="H29" s="47"/>
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
@@ -2255,7 +2242,7 @@
       <c r="AH29" s="23"/>
       <c r="AI29" s="21"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>75</v>
       </c>
@@ -2265,7 +2252,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="46"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
@@ -2294,7 +2281,7 @@
       <c r="AH30" s="23"/>
       <c r="AI30" s="21"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>74</v>
       </c>
@@ -2304,7 +2291,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="46"/>
+      <c r="H31" s="47"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
@@ -2333,7 +2320,7 @@
       <c r="AH31" s="23"/>
       <c r="AI31" s="21"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>92</v>
       </c>
@@ -2343,7 +2330,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="46"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
@@ -2372,7 +2359,7 @@
       <c r="AH32" s="23"/>
       <c r="AI32" s="21"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>48</v>
       </c>
@@ -2382,7 +2369,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="46"/>
+      <c r="H33" s="47"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
@@ -2411,7 +2398,7 @@
       <c r="AH33" s="23"/>
       <c r="AI33" s="21"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>36</v>
       </c>
@@ -2421,7 +2408,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="46"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
@@ -2452,7 +2439,7 @@
       </c>
       <c r="AI34" s="21"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>46</v>
       </c>
@@ -2462,7 +2449,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="46"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
@@ -2491,7 +2478,7 @@
       <c r="AH35" s="34"/>
       <c r="AI35" s="21"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>49</v>
       </c>
@@ -2501,7 +2488,7 @@
       <c r="E36" s="35"/>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
-      <c r="H36" s="47"/>
+      <c r="H36" s="48"/>
       <c r="I36" s="35"/>
       <c r="J36" s="35"/>
       <c r="K36" s="35"/>
@@ -2530,67 +2517,67 @@
       <c r="AH36" s="38"/>
       <c r="AI36" s="21"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H57" s="2"/>
     </row>
   </sheetData>
@@ -2611,13 +2598,13 @@
       <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.81640625" style="1" customWidth="1"/>
-    <col min="2" max="34" width="5.54296875" customWidth="1"/>
+    <col min="1" max="1" width="99.85546875" style="1" customWidth="1"/>
+    <col min="2" max="34" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2708,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>33</v>
       </c>
@@ -2733,7 +2720,7 @@
         <v>43893</v>
       </c>
       <c r="G2" s="43"/>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="46" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="43"/>
@@ -2764,7 +2751,7 @@
       <c r="AH2" s="44"/>
       <c r="AI2" s="21"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
@@ -2774,7 +2761,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="22"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="46"/>
+      <c r="H3" s="47"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
@@ -2803,7 +2790,7 @@
       <c r="AH3" s="25"/>
       <c r="AI3" s="21"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>39</v>
       </c>
@@ -2813,7 +2800,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="22"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="46"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
@@ -2842,7 +2829,7 @@
       <c r="AH4" s="25"/>
       <c r="AI4" s="21"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>40</v>
       </c>
@@ -2852,7 +2839,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="22"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="46"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
@@ -2881,7 +2868,7 @@
       <c r="AH5" s="25"/>
       <c r="AI5" s="21"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
@@ -2891,7 +2878,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="22"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="46"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
@@ -2920,7 +2907,7 @@
       <c r="AH6" s="25"/>
       <c r="AI6" s="21"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
@@ -2930,7 +2917,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="22"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="46"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -2959,7 +2946,7 @@
       <c r="AH7" s="25"/>
       <c r="AI7" s="21"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>43</v>
       </c>
@@ -2969,7 +2956,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="22"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="46"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
@@ -2998,7 +2985,7 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="21"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
@@ -3008,7 +2995,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="22"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="46"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -3037,7 +3024,7 @@
       <c r="AH9" s="25"/>
       <c r="AI9" s="21"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>45</v>
       </c>
@@ -3047,7 +3034,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="22"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="46"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
@@ -3076,7 +3063,7 @@
       <c r="AH10" s="25"/>
       <c r="AI10" s="21"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -3086,7 +3073,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="46"/>
+      <c r="H11" s="47"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
@@ -3117,7 +3104,7 @@
       <c r="AH11" s="23"/>
       <c r="AI11" s="21"/>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>51</v>
       </c>
@@ -3127,7 +3114,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="46"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -3156,7 +3143,7 @@
       <c r="AH12" s="23"/>
       <c r="AI12" s="21"/>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>52</v>
       </c>
@@ -3166,7 +3153,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="46"/>
+      <c r="H13" s="47"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -3195,7 +3182,7 @@
       <c r="AH13" s="23"/>
       <c r="AI13" s="21"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>53</v>
       </c>
@@ -3205,7 +3192,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="46"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -3234,7 +3221,7 @@
       <c r="AH14" s="23"/>
       <c r="AI14" s="21"/>
     </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>54</v>
       </c>
@@ -3244,7 +3231,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="46"/>
+      <c r="H15" s="47"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -3273,7 +3260,7 @@
       <c r="AH15" s="23"/>
       <c r="AI15" s="21"/>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -3283,7 +3270,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="46"/>
+      <c r="H16" s="47"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -3312,7 +3299,7 @@
       <c r="AH16" s="23"/>
       <c r="AI16" s="21"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>66</v>
       </c>
@@ -3322,7 +3309,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="46"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -3351,7 +3338,7 @@
       <c r="AH17" s="23"/>
       <c r="AI17" s="21"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>56</v>
       </c>
@@ -3361,7 +3348,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="46"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -3390,7 +3377,7 @@
       <c r="AH18" s="23"/>
       <c r="AI18" s="21"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>47</v>
       </c>
@@ -3400,7 +3387,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="46"/>
+      <c r="H19" s="47"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="28"/>
@@ -3429,7 +3416,7 @@
       <c r="AH19" s="23"/>
       <c r="AI19" s="21"/>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
@@ -3439,7 +3426,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="46"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
@@ -3470,7 +3457,7 @@
       <c r="AH20" s="23"/>
       <c r="AI20" s="21"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>57</v>
       </c>
@@ -3480,7 +3467,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="46"/>
+      <c r="H21" s="47"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -3509,7 +3496,7 @@
       <c r="AH21" s="23"/>
       <c r="AI21" s="21"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>58</v>
       </c>
@@ -3519,7 +3506,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="46"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
@@ -3548,7 +3535,7 @@
       <c r="AH22" s="23"/>
       <c r="AI22" s="21"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>59</v>
       </c>
@@ -3558,7 +3545,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="46"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
@@ -3587,7 +3574,7 @@
       <c r="AH23" s="23"/>
       <c r="AI23" s="21"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>60</v>
       </c>
@@ -3597,7 +3584,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="46"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
@@ -3626,7 +3613,7 @@
       <c r="AH24" s="23"/>
       <c r="AI24" s="21"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>61</v>
       </c>
@@ -3636,7 +3623,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="46"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
@@ -3665,7 +3652,7 @@
       <c r="AH25" s="23"/>
       <c r="AI25" s="21"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>62</v>
       </c>
@@ -3675,7 +3662,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="46"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
@@ -3704,7 +3691,7 @@
       <c r="AH26" s="23"/>
       <c r="AI26" s="21"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -3714,7 +3701,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="46"/>
+      <c r="H27" s="47"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
@@ -3743,7 +3730,7 @@
       <c r="AH27" s="23"/>
       <c r="AI27" s="21"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>64</v>
       </c>
@@ -3753,7 +3740,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="46"/>
+      <c r="H28" s="47"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -3782,7 +3769,7 @@
       <c r="AH28" s="23"/>
       <c r="AI28" s="21"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>65</v>
       </c>
@@ -3792,7 +3779,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="46"/>
+      <c r="H29" s="47"/>
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
@@ -3821,7 +3808,7 @@
       <c r="AH29" s="23"/>
       <c r="AI29" s="21"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>48</v>
       </c>
@@ -3831,7 +3818,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="46"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
@@ -3860,7 +3847,7 @@
       <c r="AH30" s="23"/>
       <c r="AI30" s="21"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>36</v>
       </c>
@@ -3870,7 +3857,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="46"/>
+      <c r="H31" s="47"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
@@ -3901,7 +3888,7 @@
       </c>
       <c r="AI31" s="21"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>46</v>
       </c>
@@ -3911,7 +3898,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="46"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
@@ -3940,7 +3927,7 @@
       <c r="AH32" s="34"/>
       <c r="AI32" s="21"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>50</v>
       </c>
@@ -3950,7 +3937,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="46"/>
+      <c r="H33" s="47"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
@@ -3979,7 +3966,7 @@
       <c r="AH33" s="34"/>
       <c r="AI33" s="21"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>50</v>
       </c>
@@ -3989,7 +3976,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="46"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
@@ -4018,7 +4005,7 @@
       <c r="AH34" s="34"/>
       <c r="AI34" s="21"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>50</v>
       </c>
@@ -4028,7 +4015,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="46"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
@@ -4057,7 +4044,7 @@
       <c r="AH35" s="34"/>
       <c r="AI35" s="21"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>50</v>
       </c>
@@ -4067,7 +4054,7 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="46"/>
+      <c r="H36" s="47"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
@@ -4096,7 +4083,7 @@
       <c r="AH36" s="34"/>
       <c r="AI36" s="21"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>50</v>
       </c>
@@ -4106,7 +4093,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="46"/>
+      <c r="H37" s="47"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
@@ -4135,7 +4122,7 @@
       <c r="AH37" s="34"/>
       <c r="AI37" s="21"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>50</v>
       </c>
@@ -4145,7 +4132,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="46"/>
+      <c r="H38" s="47"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
@@ -4174,7 +4161,7 @@
       <c r="AH38" s="34"/>
       <c r="AI38" s="21"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>50</v>
       </c>
@@ -4184,7 +4171,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="46"/>
+      <c r="H39" s="47"/>
       <c r="I39" s="22"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
@@ -4213,7 +4200,7 @@
       <c r="AH39" s="34"/>
       <c r="AI39" s="21"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>49</v>
       </c>
@@ -4223,7 +4210,7 @@
       <c r="E40" s="35"/>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
-      <c r="H40" s="47"/>
+      <c r="H40" s="48"/>
       <c r="I40" s="35"/>
       <c r="J40" s="35"/>
       <c r="K40" s="35"/>
@@ -4252,67 +4239,67 @@
       <c r="AH40" s="38"/>
       <c r="AI40" s="21"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H61" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on part 1 of TMA01, updated schedule with some new ideas.
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EA20C6-7554-4FFA-AB1E-614BDF11987E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEA00CA-7C8F-43A6-A085-FB12A51F0B86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>3rd Feb</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>CF5 - Produce graphs and report to show successfulness of the algorithm</t>
+  </si>
+  <si>
+    <t>CF6 - develop a feed from a sports website to pull in the latest fixtures</t>
+  </si>
+  <si>
+    <t>CF7 – develop a user interface</t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,6 +401,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF75FFB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -570,12 +588,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -584,6 +596,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,23 +936,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI65"/>
+  <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH46" sqref="A1:AH46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="102.5703125" style="1" customWidth="1"/>
     <col min="2" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="23" width="5.5703125" customWidth="1"/>
-    <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="33" width="5.5703125" customWidth="1"/>
-    <col min="34" max="34" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="75.75" x14ac:dyDescent="0.25">
@@ -1043,7 +1069,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="40" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="13"/>
@@ -1084,7 +1110,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="36"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1123,7 +1149,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="36"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -1161,7 +1187,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="36"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
@@ -1198,7 +1224,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="36"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
@@ -1236,7 +1262,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="36"/>
+      <c r="H7" s="40"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -1275,7 +1301,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="36"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -1314,7 +1340,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="36"/>
+      <c r="H9" s="40"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -1353,7 +1379,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -1392,7 +1418,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="36"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1431,7 +1457,7 @@
       <c r="E12" s="21"/>
       <c r="F12" s="4"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="36"/>
+      <c r="H12" s="40"/>
       <c r="I12" s="13"/>
       <c r="J12" s="21"/>
       <c r="K12" s="13"/>
@@ -1472,7 +1498,7 @@
         <v>43893</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="36"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -1511,7 +1537,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="23"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="36"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1549,7 +1575,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="36"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
@@ -1587,7 +1613,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="36"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="23"/>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
@@ -1625,7 +1651,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="H17" s="36"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
       <c r="K17" s="2"/>
@@ -1664,7 +1690,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="36"/>
+      <c r="H18" s="40"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="12"/>
@@ -1702,7 +1728,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="36"/>
+      <c r="H19" s="40"/>
       <c r="J19" s="33"/>
       <c r="K19" s="32"/>
       <c r="L19" s="4"/>
@@ -1740,7 +1766,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="36"/>
+      <c r="H20" s="40"/>
       <c r="I20" s="4"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
@@ -1780,7 +1806,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="36"/>
+      <c r="H21" s="40"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1819,7 +1845,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="36"/>
+      <c r="H22" s="40"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1858,7 +1884,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="36"/>
+      <c r="H23" s="40"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1896,7 +1922,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="36"/>
+      <c r="H24" s="40"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1934,7 +1960,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="36"/>
+      <c r="H25" s="40"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1972,7 +1998,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="36"/>
+      <c r="H26" s="40"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2010,7 +2036,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="36"/>
+      <c r="H27" s="40"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2047,7 +2073,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="36"/>
+      <c r="H28" s="40"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2084,7 +2110,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="36"/>
+      <c r="H29" s="40"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2119,7 +2145,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="36"/>
+      <c r="H30" s="40"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -2154,7 +2180,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="36"/>
+      <c r="H31" s="40"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2195,7 +2221,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="36"/>
+      <c r="H32" s="40"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2231,7 +2257,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="36"/>
+      <c r="H33" s="40"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2267,7 +2293,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="36"/>
+      <c r="H34" s="40"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2304,7 +2330,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="36"/>
+      <c r="H35" s="40"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2339,7 +2365,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="36"/>
+      <c r="H36" s="40"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2373,7 +2399,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="36"/>
+      <c r="H37" s="40"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2401,7 +2427,7 @@
       <c r="AI37" s="7"/>
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="4"/>
@@ -2410,7 +2436,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="36"/>
+      <c r="H38" s="40"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2429,7 +2455,7 @@
       <c r="X38" s="12"/>
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
-      <c r="AA38" s="40"/>
+      <c r="AA38" s="38"/>
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
       <c r="AD38" s="4"/>
@@ -2439,7 +2465,7 @@
       <c r="AI38" s="7"/>
     </row>
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B39" s="4"/>
@@ -2448,7 +2474,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="36"/>
+      <c r="H39" s="40"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -2467,7 +2493,7 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
-      <c r="AA39" s="40"/>
+      <c r="AA39" s="38"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="4"/>
       <c r="AD39" s="4"/>
@@ -2477,7 +2503,7 @@
       <c r="AI39" s="7"/>
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="37" t="s">
         <v>74</v>
       </c>
       <c r="B40" s="4"/>
@@ -2486,7 +2512,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="36"/>
+      <c r="H40" s="40"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2505,9 +2531,9 @@
       <c r="X40" s="12"/>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
-      <c r="AA40" s="40"/>
-      <c r="AB40" s="41"/>
-      <c r="AC40" s="41"/>
+      <c r="AA40" s="38"/>
+      <c r="AB40" s="39"/>
+      <c r="AC40" s="39"/>
       <c r="AD40" s="4"/>
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
@@ -2515,7 +2541,7 @@
       <c r="AI40" s="7"/>
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="37" t="s">
         <v>75</v>
       </c>
       <c r="B41" s="4"/>
@@ -2524,7 +2550,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="36"/>
+      <c r="H41" s="40"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -2543,16 +2569,16 @@
       <c r="X41" s="12"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
-      <c r="AB41" s="4"/>
-      <c r="AC41" s="41"/>
-      <c r="AD41" s="41"/>
+      <c r="AB41" s="39"/>
+      <c r="AC41" s="39"/>
+      <c r="AD41" s="4"/>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
       <c r="AH41" s="15"/>
       <c r="AI41" s="7"/>
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B42" s="4"/>
@@ -2561,7 +2587,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="36"/>
+      <c r="H42" s="40"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -2581,15 +2607,15 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
       <c r="AB42" s="4"/>
-      <c r="AC42" s="41"/>
-      <c r="AD42" s="41"/>
+      <c r="AC42" s="39"/>
+      <c r="AD42" s="4"/>
       <c r="AF42" s="4"/>
       <c r="AG42" s="4"/>
       <c r="AH42" s="15"/>
       <c r="AI42" s="7"/>
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B43" s="4"/>
@@ -2598,7 +2624,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="36"/>
+      <c r="H43" s="40"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2618,65 +2644,135 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
       <c r="AB43" s="4"/>
-      <c r="AC43" s="41"/>
-      <c r="AD43" s="41"/>
+      <c r="AC43" s="39"/>
+      <c r="AD43" s="4"/>
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
       <c r="AH43" s="15"/>
       <c r="AI43" s="7"/>
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4"/>
+      <c r="AD44" s="43"/>
+      <c r="AE44" s="43"/>
+      <c r="AF44" s="4"/>
+      <c r="AG44" s="4"/>
+      <c r="AH44" s="15"/>
+      <c r="AI44" s="7"/>
+    </row>
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="45"/>
+      <c r="AE45" s="45"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="15"/>
+      <c r="AI45" s="7"/>
+    </row>
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="10"/>
-      <c r="Z44" s="10"/>
-      <c r="AA44" s="10"/>
-      <c r="AB44" s="10"/>
-      <c r="AC44" s="10"/>
-      <c r="AD44" s="21"/>
-      <c r="AE44" s="21"/>
-      <c r="AF44" s="21"/>
-      <c r="AG44" s="21"/>
-      <c r="AH44" s="8">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="9"/>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="10"/>
+      <c r="AB46" s="10"/>
+      <c r="AC46" s="10"/>
+      <c r="AD46" s="21"/>
+      <c r="AE46" s="21"/>
+      <c r="AF46" s="21"/>
+      <c r="AG46" s="21"/>
+      <c r="AH46" s="8">
         <v>44088</v>
       </c>
-      <c r="AI44" s="7"/>
-    </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H45" s="5"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H46" s="5"/>
+      <c r="AI46" s="7"/>
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="5"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="5"/>
@@ -2729,12 +2825,18 @@
     <row r="64" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H65" s="2"/>
+    <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:H44"/>
+    <mergeCell ref="H2:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Literature update for TMA, schedule updated.
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEA00CA-7C8F-43A6-A085-FB12A51F0B86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E30706-73AC-4B8E-8628-57FA6B4A560D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>3rd Feb</t>
   </si>
@@ -285,10 +285,22 @@
     <t>CF5 - Produce graphs and report to show successfulness of the algorithm</t>
   </si>
   <si>
-    <t>CF6 - develop a feed from a sports website to pull in the latest fixtures</t>
-  </si>
-  <si>
-    <t>CF7 – develop a user interface</t>
+    <t>CF2 - Reflect on CF2</t>
+  </si>
+  <si>
+    <t>CF3 - Reflect on CF3</t>
+  </si>
+  <si>
+    <t>CF4 - Reflect on CF4</t>
+  </si>
+  <si>
+    <t>CF5 - Reflect on CF5</t>
+  </si>
+  <si>
+    <t>CF6 - Develop a feed from a sports website to pull in the latest fixtures</t>
+  </si>
+  <si>
+    <t>CF7 – Develop a user interface</t>
   </si>
 </sst>
 </file>
@@ -596,12 +608,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -610,6 +616,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI67"/>
+  <dimension ref="A1:AI71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH46" sqref="A1:AH46"/>
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1081,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="44" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="13"/>
@@ -1110,7 +1122,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="40"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1149,7 +1161,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="40"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -1187,7 +1199,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="40"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
@@ -1224,7 +1236,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="40"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
@@ -1262,7 +1274,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="40"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -1301,7 +1313,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="40"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -1340,7 +1352,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="40"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -1379,7 +1391,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="40"/>
+      <c r="H10" s="44"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -1418,7 +1430,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="40"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1457,7 +1469,7 @@
       <c r="E12" s="21"/>
       <c r="F12" s="4"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="40"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="13"/>
       <c r="J12" s="21"/>
       <c r="K12" s="13"/>
@@ -1498,7 +1510,7 @@
         <v>43893</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="40"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -1537,7 +1549,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="23"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="40"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1575,7 +1587,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="40"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
@@ -1613,7 +1625,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="40"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="23"/>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
@@ -1651,7 +1663,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="H17" s="40"/>
+      <c r="H17" s="44"/>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
       <c r="K17" s="2"/>
@@ -1690,7 +1702,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="40"/>
+      <c r="H18" s="44"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="12"/>
@@ -1728,7 +1740,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="40"/>
+      <c r="H19" s="44"/>
       <c r="J19" s="33"/>
       <c r="K19" s="32"/>
       <c r="L19" s="4"/>
@@ -1766,7 +1778,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="40"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="4"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
@@ -1806,7 +1818,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="40"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1845,7 +1857,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="40"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1884,7 +1896,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="40"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1922,7 +1934,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="40"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1951,8 +1963,8 @@
       <c r="AI24" s="7"/>
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>60</v>
+      <c r="A25" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1960,7 +1972,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="40"/>
+      <c r="H25" s="44"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1968,8 +1980,8 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="4"/>
+      <c r="P25" s="32"/>
+      <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
@@ -1989,8 +2001,8 @@
       <c r="AI25" s="7"/>
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>61</v>
+      <c r="A26" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1998,7 +2010,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="40"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2027,8 +2039,8 @@
       <c r="AI26" s="7"/>
     </row>
     <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>62</v>
+      <c r="A27" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2036,7 +2048,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="40"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2044,14 +2056,15 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="4"/>
+      <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
@@ -2064,8 +2077,8 @@
       <c r="AI27" s="7"/>
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>63</v>
+      <c r="A28" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2073,7 +2086,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="40"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2082,10 +2095,10 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
       <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
+      <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
@@ -2101,8 +2114,8 @@
       <c r="AI28" s="7"/>
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>64</v>
+      <c r="A29" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2110,7 +2123,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="40"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2123,7 +2136,9 @@
       <c r="R29" s="4"/>
       <c r="S29" s="34"/>
       <c r="T29" s="34"/>
+      <c r="U29" s="4"/>
       <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
       <c r="Z29" s="4"/>
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
@@ -2137,7 +2152,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2145,7 +2160,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="40"/>
+      <c r="H30" s="44"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -2156,9 +2171,9 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
+      <c r="S30" s="34"/>
       <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
+      <c r="V30" s="4"/>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
@@ -2171,8 +2186,8 @@
       <c r="AI30" s="7"/>
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>35</v>
+      <c r="A31" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2180,7 +2195,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="40"/>
+      <c r="H31" s="44"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2192,14 +2207,8 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="21"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="3">
-        <v>44019</v>
-      </c>
-      <c r="Y31" s="4"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
       <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
@@ -2212,8 +2221,8 @@
       <c r="AI31" s="7"/>
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>66</v>
+      <c r="A32" s="27" t="s">
+        <v>79</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2221,7 +2230,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="40"/>
+      <c r="H32" s="44"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2234,13 +2243,12 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="35"/>
+      <c r="U32" s="34"/>
       <c r="Z32" s="4"/>
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
@@ -2248,8 +2256,8 @@
       <c r="AI32" s="7"/>
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>67</v>
+      <c r="A33" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2257,7 +2265,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="40"/>
+      <c r="H33" s="44"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2271,12 +2279,17 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="35"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
+      <c r="X33" s="3">
+        <v>44019</v>
+      </c>
+      <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
@@ -2284,8 +2297,8 @@
       <c r="AI33" s="7"/>
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>68</v>
+      <c r="A34" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2293,7 +2306,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="40"/>
+      <c r="H34" s="44"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2307,11 +2320,10 @@
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
+      <c r="V34" s="35"/>
       <c r="W34" s="4"/>
       <c r="X34" s="35"/>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35"/>
+      <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
       <c r="AE34" s="4"/>
@@ -2321,8 +2333,8 @@
       <c r="AI34" s="7"/>
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>69</v>
+      <c r="A35" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2330,7 +2342,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="40"/>
+      <c r="H35" s="44"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2344,11 +2356,12 @@
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
+      <c r="V35" s="35"/>
       <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Z35" s="35"/>
+      <c r="X35" s="35"/>
+      <c r="Z35" s="4"/>
       <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
@@ -2356,8 +2369,8 @@
       <c r="AI35" s="7"/>
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>70</v>
+      <c r="A36" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2365,7 +2378,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="40"/>
+      <c r="H36" s="44"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2381,8 +2394,11 @@
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
+      <c r="X36" s="35"/>
+      <c r="Y36" s="35"/>
       <c r="Z36" s="35"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
       <c r="AG36" s="4"/>
@@ -2390,8 +2406,8 @@
       <c r="AI36" s="7"/>
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
-        <v>71</v>
+      <c r="A37" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2399,7 +2415,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="40"/>
+      <c r="H37" s="44"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2416,19 +2432,17 @@
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
       <c r="Z37" s="35"/>
-      <c r="AA37" s="35"/>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
+      <c r="AA37" s="4"/>
+      <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
       <c r="AH37" s="15"/>
       <c r="AI37" s="7"/>
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>72</v>
+      <c r="A38" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2436,7 +2450,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="40"/>
+      <c r="H38" s="44"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2452,21 +2466,17 @@
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
-      <c r="X38" s="12"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="38"/>
-      <c r="AB38" s="4"/>
-      <c r="AC38" s="4"/>
-      <c r="AD38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Z38" s="35"/>
+      <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
       <c r="AH38" s="15"/>
       <c r="AI38" s="7"/>
     </row>
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
-        <v>73</v>
+      <c r="A39" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2474,7 +2484,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="40"/>
+      <c r="H39" s="44"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -2490,21 +2500,20 @@
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
-      <c r="X39" s="12"/>
+      <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="38"/>
-      <c r="AB39" s="4"/>
-      <c r="AC39" s="4"/>
-      <c r="AD39" s="4"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="15"/>
       <c r="AI39" s="7"/>
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>74</v>
+      <c r="A40" s="30" t="s">
+        <v>80</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2512,7 +2521,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="40"/>
+      <c r="H40" s="44"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2528,21 +2537,20 @@
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
-      <c r="X40" s="12"/>
+      <c r="X40" s="4"/>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
-      <c r="AA40" s="38"/>
-      <c r="AB40" s="39"/>
-      <c r="AC40" s="39"/>
-      <c r="AD40" s="4"/>
+      <c r="AA40" s="35"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
       <c r="AH40" s="15"/>
       <c r="AI40" s="7"/>
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>75</v>
+      <c r="A41" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2550,7 +2558,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="40"/>
+      <c r="H41" s="44"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -2569,8 +2577,9 @@
       <c r="X41" s="12"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
-      <c r="AB41" s="39"/>
-      <c r="AC41" s="39"/>
+      <c r="AA41" s="38"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
       <c r="AD41" s="4"/>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
@@ -2579,7 +2588,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2587,7 +2596,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="40"/>
+      <c r="H42" s="44"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -2606,8 +2615,9 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
+      <c r="AA42" s="38"/>
       <c r="AB42" s="4"/>
-      <c r="AC42" s="39"/>
+      <c r="AC42" s="4"/>
       <c r="AD42" s="4"/>
       <c r="AF42" s="4"/>
       <c r="AG42" s="4"/>
@@ -2615,8 +2625,8 @@
       <c r="AI42" s="7"/>
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>77</v>
+      <c r="A43" s="37" t="s">
+        <v>74</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2624,7 +2634,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="40"/>
+      <c r="H43" s="44"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2643,7 +2653,8 @@
       <c r="X43" s="12"/>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
-      <c r="AB43" s="4"/>
+      <c r="AA43" s="38"/>
+      <c r="AB43" s="39"/>
       <c r="AC43" s="39"/>
       <c r="AD43" s="4"/>
       <c r="AF43" s="4"/>
@@ -2652,8 +2663,8 @@
       <c r="AI43" s="7"/>
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="42" t="s">
-        <v>78</v>
+      <c r="A44" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2661,7 +2672,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="40"/>
+      <c r="H44" s="44"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2680,18 +2691,17 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
-      <c r="AB44" s="4"/>
-      <c r="AC44" s="4"/>
-      <c r="AD44" s="43"/>
-      <c r="AE44" s="43"/>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="4"/>
       <c r="AF44" s="4"/>
       <c r="AG44" s="4"/>
       <c r="AH44" s="15"/>
       <c r="AI44" s="7"/>
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
-        <v>79</v>
+      <c r="A45" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2699,7 +2709,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="40"/>
+      <c r="H45" s="44"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -2719,110 +2729,247 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
       <c r="AB45" s="4"/>
-      <c r="AC45" s="4"/>
-      <c r="AD45" s="45"/>
-      <c r="AE45" s="45"/>
+      <c r="AC45" s="39"/>
+      <c r="AD45" s="4"/>
       <c r="AF45" s="4"/>
       <c r="AG45" s="4"/>
       <c r="AH45" s="15"/>
       <c r="AI45" s="7"/>
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="39"/>
+      <c r="AD46" s="4"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="15"/>
+      <c r="AI46" s="7"/>
+    </row>
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="12"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="39"/>
+      <c r="AD47" s="4"/>
+      <c r="AF47" s="4"/>
+      <c r="AG47" s="4"/>
+      <c r="AH47" s="15"/>
+      <c r="AI47" s="7"/>
+    </row>
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="12"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="41"/>
+      <c r="AE48" s="41"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="15"/>
+      <c r="AI48" s="7"/>
+    </row>
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="12"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="43"/>
+      <c r="AE49" s="43"/>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="15"/>
+      <c r="AI49" s="7"/>
+    </row>
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="10"/>
-      <c r="Z46" s="10"/>
-      <c r="AA46" s="10"/>
-      <c r="AB46" s="10"/>
-      <c r="AC46" s="10"/>
-      <c r="AD46" s="21"/>
-      <c r="AE46" s="21"/>
-      <c r="AF46" s="21"/>
-      <c r="AG46" s="21"/>
-      <c r="AH46" s="8">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="10"/>
+      <c r="Z50" s="10"/>
+      <c r="AA50" s="10"/>
+      <c r="AB50" s="10"/>
+      <c r="AC50" s="10"/>
+      <c r="AD50" s="21"/>
+      <c r="AE50" s="21"/>
+      <c r="AF50" s="21"/>
+      <c r="AG50" s="21"/>
+      <c r="AH50" s="8">
         <v>44088</v>
       </c>
-      <c r="AI46" s="7"/>
-    </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H47" s="5"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI50" s="7"/>
+    </row>
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2831,12 +2978,24 @@
     <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H67" s="2"/>
+    <row r="67" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="H2:H50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Researched KNN and K-Means, updated schedule again slightly, more work on TMA01 and added references based on research into where I can find premier league data.
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E30706-73AC-4B8E-8628-57FA6B4A560D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B585CD3-720A-4E46-A653-8CB2C74F77D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18740" yWindow="2280" windowWidth="16710" windowHeight="12940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -951,23 +951,23 @@
   <dimension ref="A1:AI71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="102.5703125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="23" width="5.5703125" customWidth="1"/>
-    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="33" width="5.5703125" customWidth="1"/>
-    <col min="34" max="34" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.54296875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="5.54296875" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.54296875" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="5.54296875" customWidth="1"/>
+    <col min="24" max="24" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="33" width="5.54296875" customWidth="1"/>
+    <col min="34" max="34" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="75" x14ac:dyDescent="0.35">
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>42</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="AH2" s="14"/>
       <c r="AI2" s="7"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>43</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="AH3" s="14"/>
       <c r="AI3" s="7"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>44</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="AH4" s="14"/>
       <c r="AI4" s="7"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>45</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="AH5" s="14"/>
       <c r="AI5" s="7"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>46</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="AH6" s="14"/>
       <c r="AI6" s="7"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>38</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="AH7" s="14"/>
       <c r="AI7" s="7"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>47</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="AH8" s="14"/>
       <c r="AI8" s="7"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="AH9" s="14"/>
       <c r="AI9" s="7"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>49</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="AH10" s="14"/>
       <c r="AI10" s="7"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>50</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="AH11" s="14"/>
       <c r="AI11" s="7"/>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="AH12" s="14"/>
       <c r="AI12" s="7"/>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="AH13" s="14"/>
       <c r="AI13" s="7"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>52</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="AH14" s="15"/>
       <c r="AI14" s="7"/>
     </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="AH15" s="15"/>
       <c r="AI15" s="7"/>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>53</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="AH16" s="15"/>
       <c r="AI16" s="7"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>54</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="AH17" s="15"/>
       <c r="AI17" s="7"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>51</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="AH18" s="15"/>
       <c r="AI18" s="16"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>55</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="AH19" s="15"/>
       <c r="AI19" s="16"/>
     </row>
-    <row r="20" spans="1:35" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>34</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="AG20" s="4"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>56</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="AH21" s="15"/>
       <c r="AI21" s="16"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>57</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="AH22" s="15"/>
       <c r="AI22" s="7"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>58</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="AH23" s="15"/>
       <c r="AI23" s="7"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
         <v>59</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="AH24" s="15"/>
       <c r="AI24" s="7"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>78</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="AH25" s="15"/>
       <c r="AI25" s="7"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
         <v>60</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="AH26" s="15"/>
       <c r="AI26" s="7"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>61</v>
       </c>
@@ -2076,7 +2076,7 @@
       <c r="AH27" s="15"/>
       <c r="AI27" s="7"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27" t="s">
         <v>62</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="AH28" s="15"/>
       <c r="AI28" s="7"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="s">
         <v>63</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="AH29" s="15"/>
       <c r="AI29" s="7"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27" t="s">
         <v>64</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="AH30" s="15"/>
       <c r="AI30" s="7"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="27" t="s">
         <v>65</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="AH31" s="15"/>
       <c r="AI31" s="7"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="27" t="s">
         <v>79</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="AH32" s="15"/>
       <c r="AI32" s="7"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>35</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="AH33" s="15"/>
       <c r="AI33" s="7"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>66</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="AH34" s="15"/>
       <c r="AI34" s="7"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>67</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="AH35" s="15"/>
       <c r="AI35" s="7"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="31" t="s">
         <v>68</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="AH36" s="15"/>
       <c r="AI36" s="7"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="31" t="s">
         <v>69</v>
       </c>
@@ -2440,7 +2440,7 @@
       <c r="AH37" s="15"/>
       <c r="AI37" s="7"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="30" t="s">
         <v>70</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="AH38" s="15"/>
       <c r="AI38" s="7"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="30" t="s">
         <v>71</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="AH39" s="15"/>
       <c r="AI39" s="7"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="30" t="s">
         <v>80</v>
       </c>
@@ -2548,7 +2548,7 @@
       <c r="AH40" s="15"/>
       <c r="AI40" s="7"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
         <v>72</v>
       </c>
@@ -2586,7 +2586,7 @@
       <c r="AH41" s="15"/>
       <c r="AI41" s="7"/>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
         <v>73</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="AH42" s="15"/>
       <c r="AI42" s="7"/>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="37" t="s">
         <v>74</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="AH43" s="15"/>
       <c r="AI43" s="7"/>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="37" t="s">
         <v>75</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="AH44" s="15"/>
       <c r="AI44" s="7"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="36" t="s">
         <v>76</v>
       </c>
@@ -2736,7 +2736,7 @@
       <c r="AH45" s="15"/>
       <c r="AI45" s="7"/>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36" t="s">
         <v>77</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="AH46" s="15"/>
       <c r="AI46" s="7"/>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="36" t="s">
         <v>81</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="AH47" s="15"/>
       <c r="AI47" s="7"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="40" t="s">
         <v>82</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="AH48" s="15"/>
       <c r="AI48" s="7"/>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="42" t="s">
         <v>83</v>
       </c>
@@ -2886,7 +2886,7 @@
       <c r="AH49" s="15"/>
       <c r="AI49" s="7"/>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
         <v>36</v>
       </c>
@@ -2927,70 +2927,70 @@
       </c>
       <c r="AI50" s="7"/>
     </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H71" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further work done on TMA01, project journal updated. Another update to schedule and research into similiar projects done
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Dev\Python\Projects\UniProject\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B585CD3-720A-4E46-A653-8CB2C74F77D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5551B0C-CF1E-4D8A-9962-07932AF687D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18740" yWindow="2280" windowWidth="16710" windowHeight="12940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -951,23 +951,23 @@
   <dimension ref="A1:AI71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.54296875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="5.54296875" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.54296875" customWidth="1"/>
-    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="23" width="5.54296875" customWidth="1"/>
-    <col min="24" max="24" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="33" width="5.54296875" customWidth="1"/>
-    <col min="34" max="34" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.5703125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="23" width="5.5703125" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="33" width="5.5703125" customWidth="1"/>
+    <col min="34" max="34" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="75.75" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>42</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="AH2" s="14"/>
       <c r="AI2" s="7"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>43</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="AH3" s="14"/>
       <c r="AI3" s="7"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>44</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="AH4" s="14"/>
       <c r="AI4" s="7"/>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>45</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="AH5" s="14"/>
       <c r="AI5" s="7"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>46</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="AH6" s="14"/>
       <c r="AI6" s="7"/>
     </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>38</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="AH7" s="14"/>
       <c r="AI7" s="7"/>
     </row>
-    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>47</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="AH8" s="14"/>
       <c r="AI8" s="7"/>
     </row>
-    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="AH9" s="14"/>
       <c r="AI9" s="7"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>49</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="AH10" s="14"/>
       <c r="AI10" s="7"/>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>50</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="AH11" s="14"/>
       <c r="AI11" s="7"/>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="AH12" s="14"/>
       <c r="AI12" s="7"/>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="AH13" s="14"/>
       <c r="AI13" s="7"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>52</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="AH14" s="15"/>
       <c r="AI14" s="7"/>
     </row>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="AH15" s="15"/>
       <c r="AI15" s="7"/>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>53</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="AH16" s="15"/>
       <c r="AI16" s="7"/>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>54</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="AH17" s="15"/>
       <c r="AI17" s="7"/>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>51</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="AH18" s="15"/>
       <c r="AI18" s="16"/>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>55</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="AH19" s="15"/>
       <c r="AI19" s="16"/>
     </row>
-    <row r="20" spans="1:35" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>34</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="AG20" s="4"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>56</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="AH21" s="15"/>
       <c r="AI21" s="16"/>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>57</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="AH22" s="15"/>
       <c r="AI22" s="7"/>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>58</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="AH23" s="15"/>
       <c r="AI23" s="7"/>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>59</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="AH24" s="15"/>
       <c r="AI24" s="7"/>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>78</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="AH25" s="15"/>
       <c r="AI25" s="7"/>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>60</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="AH26" s="15"/>
       <c r="AI26" s="7"/>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>61</v>
       </c>
@@ -2076,7 +2076,7 @@
       <c r="AH27" s="15"/>
       <c r="AI27" s="7"/>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>62</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="AH28" s="15"/>
       <c r="AI28" s="7"/>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>63</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="AH29" s="15"/>
       <c r="AI29" s="7"/>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>64</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="AH30" s="15"/>
       <c r="AI30" s="7"/>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>65</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="AH31" s="15"/>
       <c r="AI31" s="7"/>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>79</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="AH32" s="15"/>
       <c r="AI32" s="7"/>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>35</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="AH33" s="15"/>
       <c r="AI33" s="7"/>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>66</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="AH34" s="15"/>
       <c r="AI34" s="7"/>
     </row>
-    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>67</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="AH35" s="15"/>
       <c r="AI35" s="7"/>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>68</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="AH36" s="15"/>
       <c r="AI36" s="7"/>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>69</v>
       </c>
@@ -2440,7 +2440,7 @@
       <c r="AH37" s="15"/>
       <c r="AI37" s="7"/>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>70</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="AH38" s="15"/>
       <c r="AI38" s="7"/>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>71</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="AH39" s="15"/>
       <c r="AI39" s="7"/>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>80</v>
       </c>
@@ -2548,7 +2548,7 @@
       <c r="AH40" s="15"/>
       <c r="AI40" s="7"/>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>72</v>
       </c>
@@ -2586,7 +2586,7 @@
       <c r="AH41" s="15"/>
       <c r="AI41" s="7"/>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
         <v>73</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="AH42" s="15"/>
       <c r="AI42" s="7"/>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
         <v>74</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="AH43" s="15"/>
       <c r="AI43" s="7"/>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
         <v>75</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="AH44" s="15"/>
       <c r="AI44" s="7"/>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
         <v>76</v>
       </c>
@@ -2736,7 +2736,7 @@
       <c r="AH45" s="15"/>
       <c r="AI45" s="7"/>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
         <v>77</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="AH46" s="15"/>
       <c r="AI46" s="7"/>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
         <v>81</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="AH47" s="15"/>
       <c r="AI47" s="7"/>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
         <v>82</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="AH48" s="15"/>
       <c r="AI48" s="7"/>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="42" t="s">
         <v>83</v>
       </c>
@@ -2886,7 +2886,7 @@
       <c r="AH49" s="15"/>
       <c r="AI49" s="7"/>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>36</v>
       </c>
@@ -2927,70 +2927,70 @@
       </c>
       <c r="AI50" s="7"/>
     </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H71" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small update to schedule
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5551B0C-CF1E-4D8A-9962-07932AF687D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BC2927-9C1D-44EE-A82A-4B982B3AC414}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,9 +1703,8 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="44"/>
-      <c r="J18" s="32"/>
       <c r="K18" s="32"/>
-      <c r="L18" s="12"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1741,10 +1740,8 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="44"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="33"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -1780,7 +1777,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="44"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="21"/>
+      <c r="J20" s="4"/>
       <c r="K20" s="21"/>
       <c r="L20" s="3">
         <v>43935</v>

</xml_diff>

<commit_message>
Research into random forest algorithm. Update to schedule
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BC2927-9C1D-44EE-A82A-4B982B3AC414}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081D4934-52D2-49B8-A81E-D75F96CF4C5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>3rd Feb</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>CF7 – Develop a user interface</t>
+  </si>
+  <si>
+    <t>Write LEPSI review</t>
   </si>
 </sst>
 </file>
@@ -948,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI71"/>
+  <dimension ref="A1:AI72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,20 +1582,20 @@
       <c r="AI14" s="7"/>
     </row>
     <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>40</v>
+      <c r="A15" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="44"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="23"/>
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="21"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1604,7 +1607,7 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="21"/>
+      <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
@@ -1618,16 +1621,16 @@
     </row>
     <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="4"/>
       <c r="H16" s="44"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="2"/>
       <c r="L16" s="12"/>
       <c r="M16" s="4"/>
@@ -1655,8 +1658,8 @@
       <c r="AI16" s="7"/>
     </row>
     <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>54</v>
+      <c r="A17" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1664,8 +1667,8 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="H17" s="44"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="2"/>
       <c r="L17" s="12"/>
       <c r="M17" s="4"/>
@@ -1690,7 +1693,7 @@
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
       <c r="AH17" s="15"/>
-      <c r="AI17" s="7"/>
+      <c r="AI17" s="16"/>
     </row>
     <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
@@ -1805,23 +1808,22 @@
       <c r="AG20" s="4"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>56</v>
+    <row r="21" spans="1:35" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21"/>
       <c r="G21" s="4"/>
       <c r="H21" s="44"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
@@ -1832,7 +1834,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
+      <c r="Y21" s="21"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
@@ -1842,11 +1844,10 @@
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="15"/>
-      <c r="AI21" s="16"/>
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1858,10 +1859,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
+      <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -1881,11 +1882,11 @@
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
       <c r="AH22" s="15"/>
-      <c r="AI22" s="7"/>
+      <c r="AI22" s="16"/>
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>58</v>
+      <c r="A23" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1901,6 +1902,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
+      <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -1923,7 +1925,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1937,9 +1939,9 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="N24" s="32"/>
       <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
+      <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
@@ -1961,7 +1963,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1976,7 +1978,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
+      <c r="O25" s="32"/>
       <c r="P25" s="32"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
@@ -1998,8 +2000,8 @@
       <c r="AI25" s="7"/>
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>60</v>
+      <c r="A26" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2015,8 +2017,8 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="4"/>
+      <c r="P26" s="32"/>
+      <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
@@ -2036,8 +2038,8 @@
       <c r="AI26" s="7"/>
     </row>
     <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>61</v>
+      <c r="A27" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2074,8 +2076,8 @@
       <c r="AI27" s="7"/>
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>62</v>
+      <c r="A28" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2091,14 +2093,15 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="4"/>
+      <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
@@ -2111,8 +2114,8 @@
       <c r="AI28" s="7"/>
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>63</v>
+      <c r="A29" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2129,10 +2132,10 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
       <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
+      <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
@@ -2148,8 +2151,8 @@
       <c r="AI29" s="7"/>
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>64</v>
+      <c r="A30" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2170,7 +2173,9 @@
       <c r="R30" s="4"/>
       <c r="S30" s="34"/>
       <c r="T30" s="34"/>
+      <c r="U30" s="4"/>
       <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
@@ -2184,7 +2189,7 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2203,9 +2208,9 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
+      <c r="S31" s="34"/>
       <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
+      <c r="V31" s="4"/>
       <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
@@ -2219,7 +2224,7 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2239,7 +2244,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
+      <c r="T32" s="34"/>
       <c r="U32" s="34"/>
       <c r="Z32" s="4"/>
       <c r="AA32" s="4"/>
@@ -2253,8 +2258,8 @@
       <c r="AI32" s="7"/>
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>35</v>
+      <c r="A33" s="27" t="s">
+        <v>79</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2275,13 +2280,7 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="3">
-        <v>44019</v>
-      </c>
-      <c r="Y33" s="4"/>
+      <c r="U33" s="34"/>
       <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
@@ -2294,8 +2293,8 @@
       <c r="AI33" s="7"/>
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>66</v>
+      <c r="A34" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2317,12 +2316,17 @@
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="35"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="3">
+        <v>44019</v>
+      </c>
+      <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
@@ -2330,8 +2334,8 @@
       <c r="AI34" s="7"/>
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>67</v>
+      <c r="A35" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2366,8 +2370,8 @@
       <c r="AI35" s="7"/>
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>68</v>
+      <c r="A36" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2389,11 +2393,10 @@
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
+      <c r="V36" s="35"/>
       <c r="W36" s="4"/>
       <c r="X36" s="35"/>
-      <c r="Y36" s="35"/>
-      <c r="Z36" s="35"/>
+      <c r="Z36" s="4"/>
       <c r="AA36" s="4"/>
       <c r="AB36" s="4"/>
       <c r="AE36" s="4"/>
@@ -2404,7 +2407,7 @@
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2428,9 +2431,11 @@
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
+      <c r="X37" s="35"/>
+      <c r="Y37" s="35"/>
       <c r="Z37" s="35"/>
       <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
@@ -2438,8 +2443,8 @@
       <c r="AI37" s="7"/>
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
-        <v>70</v>
+      <c r="A38" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2465,6 +2470,7 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Z38" s="35"/>
+      <c r="AA38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
@@ -2473,7 +2479,7 @@
     </row>
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2498,11 +2504,8 @@
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
       <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
+      <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="15"/>
@@ -2510,7 +2513,7 @@
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2536,7 +2539,7 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
+      <c r="Z40" s="35"/>
       <c r="AA40" s="35"/>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
@@ -2546,8 +2549,8 @@
       <c r="AI40" s="7"/>
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>72</v>
+      <c r="A41" s="30" t="s">
+        <v>80</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2571,13 +2574,12 @@
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
-      <c r="X41" s="12"/>
+      <c r="X41" s="4"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
-      <c r="AA41" s="38"/>
-      <c r="AB41" s="4"/>
-      <c r="AC41" s="4"/>
-      <c r="AD41" s="4"/>
+      <c r="AA41" s="35"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
       <c r="AH41" s="15"/>
@@ -2585,7 +2587,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2622,8 +2624,8 @@
       <c r="AI42" s="7"/>
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
-        <v>74</v>
+      <c r="A43" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2651,8 +2653,8 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
       <c r="AA43" s="38"/>
-      <c r="AB43" s="39"/>
-      <c r="AC43" s="39"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
       <c r="AD43" s="4"/>
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
@@ -2661,7 +2663,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2688,6 +2690,7 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
+      <c r="AA44" s="38"/>
       <c r="AB44" s="39"/>
       <c r="AC44" s="39"/>
       <c r="AD44" s="4"/>
@@ -2697,8 +2700,8 @@
       <c r="AI44" s="7"/>
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
-        <v>76</v>
+      <c r="A45" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2725,7 +2728,7 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
-      <c r="AB45" s="4"/>
+      <c r="AB45" s="39"/>
       <c r="AC45" s="39"/>
       <c r="AD45" s="4"/>
       <c r="AF45" s="4"/>
@@ -2735,7 +2738,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2772,7 +2775,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2808,8 +2811,8 @@
       <c r="AI47" s="7"/>
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="40" t="s">
-        <v>82</v>
+      <c r="A48" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2837,17 +2840,16 @@
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
       <c r="AB48" s="4"/>
-      <c r="AC48" s="4"/>
-      <c r="AD48" s="41"/>
-      <c r="AE48" s="41"/>
+      <c r="AC48" s="39"/>
+      <c r="AD48" s="4"/>
       <c r="AF48" s="4"/>
       <c r="AG48" s="4"/>
       <c r="AH48" s="15"/>
       <c r="AI48" s="7"/>
     </row>
     <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="42" t="s">
-        <v>83</v>
+      <c r="A49" s="40" t="s">
+        <v>82</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2876,62 +2878,97 @@
       <c r="Z49" s="4"/>
       <c r="AB49" s="4"/>
       <c r="AC49" s="4"/>
-      <c r="AD49" s="43"/>
-      <c r="AE49" s="43"/>
+      <c r="AD49" s="41"/>
+      <c r="AE49" s="41"/>
       <c r="AF49" s="4"/>
       <c r="AG49" s="4"/>
       <c r="AH49" s="15"/>
       <c r="AI49" s="7"/>
     </row>
     <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="43"/>
+      <c r="AE50" s="43"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="15"/>
+      <c r="AI50" s="7"/>
+    </row>
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="10"/>
-      <c r="Z50" s="10"/>
-      <c r="AA50" s="10"/>
-      <c r="AB50" s="10"/>
-      <c r="AC50" s="10"/>
-      <c r="AD50" s="21"/>
-      <c r="AE50" s="21"/>
-      <c r="AF50" s="21"/>
-      <c r="AG50" s="21"/>
-      <c r="AH50" s="8">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="10"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="10"/>
+      <c r="AC51" s="10"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="21"/>
+      <c r="AF51" s="21"/>
+      <c r="AG51" s="21"/>
+      <c r="AH51" s="8">
         <v>44088</v>
       </c>
-      <c r="AI50" s="7"/>
-    </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H51" s="5"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="AI51" s="7"/>
     </row>
     <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H52" s="5"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
     </row>
     <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H53" s="5"/>
@@ -2987,12 +3024,15 @@
     <row r="70" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H71" s="2"/>
+    <row r="71" spans="8:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:H50"/>
+    <mergeCell ref="H2:H51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Work on TMA03 and updates to schedule/project journal
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Dev\Python\Projects\UniProject\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AA2CFD-13C6-48E9-B822-221890FF11A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A4BCE3-06CF-4E9D-8603-505D7CE2852F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1365" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC41" sqref="AC41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,7 +2286,7 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
+      <c r="W33" s="34"/>
       <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
@@ -2321,7 +2321,7 @@
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
-      <c r="U34" s="34"/>
+      <c r="W34" s="34"/>
       <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
@@ -2356,9 +2356,8 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
+      <c r="U35" s="21"/>
       <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
       <c r="X35" s="3">
         <v>44019</v>
       </c>
@@ -2398,8 +2397,7 @@
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
-      <c r="V36" s="35"/>
-      <c r="W36" s="4"/>
+      <c r="W36" s="35"/>
       <c r="X36" s="35"/>
       <c r="Z36" s="4"/>
       <c r="AA36" s="4"/>
@@ -2434,8 +2432,7 @@
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
-      <c r="V37" s="35"/>
-      <c r="W37" s="4"/>
+      <c r="W37" s="35"/>
       <c r="X37" s="35"/>
       <c r="Z37" s="4"/>
       <c r="AA37" s="4"/>
@@ -2731,10 +2728,9 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
-      <c r="AA45" s="38"/>
       <c r="AB45" s="39"/>
       <c r="AC45" s="39"/>
-      <c r="AD45" s="4"/>
+      <c r="AD45" s="38"/>
       <c r="AF45" s="4"/>
       <c r="AG45" s="4"/>
       <c r="AH45" s="15"/>
@@ -2769,9 +2765,8 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
-      <c r="AB46" s="39"/>
-      <c r="AC46" s="39"/>
-      <c r="AD46" s="4"/>
+      <c r="AD46" s="39"/>
+      <c r="AE46" s="39"/>
       <c r="AF46" s="4"/>
       <c r="AG46" s="4"/>
       <c r="AH46" s="15"/>
@@ -2807,8 +2802,8 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
       <c r="AB47" s="4"/>
-      <c r="AC47" s="39"/>
       <c r="AD47" s="4"/>
+      <c r="AE47" s="39"/>
       <c r="AF47" s="4"/>
       <c r="AG47" s="4"/>
       <c r="AH47" s="15"/>
@@ -2844,8 +2839,8 @@
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
       <c r="AB48" s="4"/>
-      <c r="AC48" s="39"/>
       <c r="AD48" s="4"/>
+      <c r="AE48" s="39"/>
       <c r="AF48" s="4"/>
       <c r="AG48" s="4"/>
       <c r="AH48" s="15"/>
@@ -2881,8 +2876,8 @@
       <c r="Y49" s="4"/>
       <c r="Z49" s="4"/>
       <c r="AB49" s="4"/>
-      <c r="AC49" s="39"/>
       <c r="AD49" s="4"/>
+      <c r="AE49" s="39"/>
       <c r="AF49" s="4"/>
       <c r="AG49" s="4"/>
       <c r="AH49" s="15"/>
@@ -2919,9 +2914,8 @@
       <c r="Z50" s="4"/>
       <c r="AB50" s="4"/>
       <c r="AC50" s="4"/>
-      <c r="AD50" s="41"/>
       <c r="AE50" s="41"/>
-      <c r="AF50" s="4"/>
+      <c r="AF50" s="41"/>
       <c r="AG50" s="4"/>
       <c r="AH50" s="15"/>
       <c r="AI50" s="7"/>
@@ -2957,9 +2951,8 @@
       <c r="Z51" s="4"/>
       <c r="AB51" s="4"/>
       <c r="AC51" s="4"/>
-      <c r="AD51" s="43"/>
       <c r="AE51" s="43"/>
-      <c r="AF51" s="4"/>
+      <c r="AF51" s="43"/>
       <c r="AG51" s="4"/>
       <c r="AH51" s="15"/>
       <c r="AI51" s="7"/>

</xml_diff>